<commit_message>
replacing JS libraries with CDNs
</commit_message>
<xml_diff>
--- a/ressources/Modèle-audit-SEO(1).xlsx
+++ b/ressources/Modèle-audit-SEO(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertr\Documents\Tutorials\OpenClassRooms\projects\project_4\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E1A2C7-3F9E-4357-96B6-D22C6C840710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EDB9FD-89F0-4EFA-AE26-5B917D4C212D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Catégorie</t>
   </si>
@@ -120,9 +120,6 @@
     <t xml:space="preserve">Risque de pénalité </t>
   </si>
   <si>
-    <t>Ne pas mettre de texte caché avec des mots clés</t>
-  </si>
-  <si>
     <t>Meta robot</t>
   </si>
   <si>
@@ -157,6 +154,27 @@
   </si>
   <si>
     <t>Meta OG (social media)</t>
+  </si>
+  <si>
+    <t>Ne pas mettre de texte caché avec des mots clés, ou dans les attributs alt des images</t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/seo-balise-alt-images/</t>
+  </si>
+  <si>
+    <t>nom de page non-explicite</t>
+  </si>
+  <si>
+    <t>La page de contact est nommée page-2</t>
+  </si>
+  <si>
+    <t>Donner un nom de page adapté pour l'URL</t>
+  </si>
+  <si>
+    <t>Modifier "page2" par "contact"</t>
+  </si>
+  <si>
+    <t>https://www.keycdn.com/blog/why-use-a-cdn#:~:text=Faster%20performance%20and%20lower%20latency,-Of%20course%2C%20the&amp;text=Using%20a%20CDN%20allows%20us,both%20static%20and%20dynamic%20content.</t>
   </si>
 </sst>
 </file>
@@ -470,7 +488,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -542,10 +560,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -565,10 +583,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -576,13 +594,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,10 +627,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -607,13 +641,13 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -655,19 +689,22 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -676,7 +713,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -685,7 +722,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -701,18 +738,21 @@
       <c r="E21" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1684,6 +1724,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F15" r:id="rId1" xr:uid="{AEAAEFCC-9869-477D-B4F3-55889090F11E}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{A5C63F03-87F7-4C5F-B030-A0CBB1D1C99C}"/>
+    <hyperlink ref="F21" r:id="rId3" location=":~:text=Faster%20performance%20and%20lower%20latency,-Of%20course%2C%20the&amp;text=Using%20a%20CDN%20allows%20us,both%20static%20and%20dynamic%20content." xr:uid="{D8192039-F054-40DC-9D1E-6D84B328CCD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
replacing CSS libraries with CDNs
</commit_message>
<xml_diff>
--- a/ressources/Modèle-audit-SEO(1).xlsx
+++ b/ressources/Modèle-audit-SEO(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertr\Documents\Tutorials\OpenClassRooms\projects\project_4\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EDB9FD-89F0-4EFA-AE26-5B917D4C212D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6971EC2-633A-4885-9EC3-FD3F94E5BF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Catégorie</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>https://www.keycdn.com/blog/why-use-a-cdn#:~:text=Faster%20performance%20and%20lower%20latency,-Of%20course%2C%20the&amp;text=Using%20a%20CDN%20allows%20us,both%20static%20and%20dynamic%20content.</t>
+  </si>
+  <si>
+    <t>Use WebP format and adaptive resolutions</t>
+  </si>
+  <si>
+    <t>https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>Ajout @font-display:swap</t>
+  </si>
+  <si>
+    <t>https://web.dev/font-display/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -720,7 +732,12 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -744,7 +761,17 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>